<commit_message>
Some further tweaks to the model
</commit_message>
<xml_diff>
--- a/02-keyopatra-project/CAD resources/Rigel spreadsheet.xlsx
+++ b/02-keyopatra-project/CAD resources/Rigel spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\keyboards\02-keyopatra-project\CAD resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicholasWilson\Source\keyboards\02-keyopatra-project\CAD resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6F3AE3-9CD3-46F6-9EA7-0EF680FA2DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CB4B26-D37B-460E-96EF-4C743ADC0F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="23232" windowHeight="25296" xr2:uid="{32EE4ECE-299D-4BED-919A-5106D64CC162}"/>
+    <workbookView xWindow="9600" yWindow="5510" windowWidth="28800" windowHeight="15370" activeTab="3" xr2:uid="{32EE4ECE-299D-4BED-919A-5106D64CC162}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
   <si>
     <t>Thoughts on metals for keyboard plate</t>
   </si>
@@ -357,13 +357,21 @@
   <si>
     <t>Amoeba Single-Switch PCB?</t>
   </si>
+  <si>
+    <t>Convexity:</t>
+  </si>
+  <si>
+    <t>Radius:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="General&quot; rad&quot;"/>
+    <numFmt numFmtId="165" formatCode="General&quot; mm&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -419,7 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -427,6 +435,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -493,9 +503,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -533,7 +543,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -639,7 +649,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -781,7 +791,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -791,19 +801,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7E0C16-8865-409D-A480-46129CE2CEEA}">
   <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -811,7 +821,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="2:5" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -825,7 +835,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -836,7 +846,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -850,7 +860,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -864,7 +874,7 @@
         <v>7300</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -878,7 +888,7 @@
         <v>7850</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -892,7 +902,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -906,7 +916,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -920,13 +930,13 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -934,17 +944,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>23</v>
       </c>
@@ -971,20 +981,20 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="40.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>39</v>
       </c>
@@ -998,7 +1008,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>27</v>
       </c>
@@ -1012,7 +1022,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1026,7 +1036,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
@@ -1034,7 +1044,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -1042,7 +1052,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>31</v>
       </c>
@@ -1050,7 +1060,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -1061,7 +1071,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
@@ -1069,7 +1079,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>35</v>
       </c>
@@ -1077,7 +1087,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>48</v>
       </c>
@@ -1085,7 +1095,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>53</v>
       </c>
@@ -1093,13 +1103,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>64</v>
       </c>
@@ -1110,7 +1120,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>70</v>
       </c>
@@ -1118,7 +1128,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>78</v>
       </c>
@@ -1126,12 +1136,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>77</v>
       </c>
@@ -1161,67 +1171,67 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -1236,18 +1246,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15110F8F-67DA-46BD-B8B2-C9615236E7CE}">
-  <dimension ref="B2:F27"/>
+  <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>13</v>
       </c>
@@ -1261,7 +1272,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -1272,7 +1283,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1286,62 +1297,80 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="5">
+        <f>15*PI()/180</f>
+        <v>0.26179938779914941</v>
+      </c>
+      <c r="G12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="6">
+        <f>C4/2/SIN(F12/2)</f>
+        <v>72.973859407022218</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <f>ASIN(19/(2*75))*2/(2*PI())*360</f>
+        <v>14.554027753139177</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>85</v>
       </c>
@@ -1349,7 +1378,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>86</v>
       </c>
@@ -1357,7 +1386,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>87</v>
       </c>
@@ -1365,7 +1394,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>88</v>
       </c>
@@ -1373,7 +1402,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>89</v>
       </c>
@@ -1383,6 +1412,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>